<commit_message>
Add summary data to A1-report
</commit_message>
<xml_diff>
--- a/NANO_KAFFEE_GmbH_YYYY_MM_Röstprotokoll_Beleg_zu_Abtl.1.xlsx
+++ b/NANO_KAFFEE_GmbH_YYYY_MM_Röstprotokoll_Beleg_zu_Abtl.1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">NANO KAFFEE GmbH</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg</t>
   </si>
   <si>
     <t xml:space="preserve">Abtl.1</t>
@@ -101,6 +104,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -188,60 +192,56 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -431,436 +431,461 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17:F17"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="14.65" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C8" s="8"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="10" t="n">
+        <f aca="false">SUM(D10:D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="C18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C20" s="11"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="11"/>
+      <c r="F18" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D21" s="8"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D22" s="5"/>
-      <c r="E22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
+      <c r="D22" s="6"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C23" s="5"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="3"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C24" s="5"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="3"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="4"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C25" s="5"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="13"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="4"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C26" s="5"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="13"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="12"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D27" s="1"/>
-      <c r="E27" s="13"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-    </row>
-    <row r="1048422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="12"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D28" s="2"/>
+      <c r="E28" s="12"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+    </row>
     <row r="1048423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>